<commit_message>
multiple updates for VCNmodel
</commit_message>
<xml_diff>
--- a/MorphologyData/Dendrite Quality and Surface Areas_comparisons_pbm_15Mar2019_v2.xlsx
+++ b/MorphologyData/Dendrite Quality and Surface Areas_comparisons_pbm_15Mar2019_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbmanis/Desktop/Python/VCNModel/VCN_Cells/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbmanis/Desktop/Python/VCNModel/MorphologyData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67070154-6F59-394D-A9B0-0A0D9BD8C214}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47ECF12-E3C5-1940-ABF0-AAC25461565C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21020" yWindow="1940" windowWidth="29840" windowHeight="19680" tabRatio="995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -476,7 +476,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="__Anonymous_Sheet_DB__2" displayName="__Anonymous_Sheet_DB__2" ref="B20:B28" headerRowCount="0" totalsRowShown="0">
-  <sortState ref="B20:B28">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B20:B28">
     <sortCondition descending="1" ref="B21:B29"/>
   </sortState>
   <tableColumns count="1">
@@ -786,14 +786,14 @@
   <dimension ref="A1:AC55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="18"/>
+    <col min="6" max="6" width="14.6640625" style="18" customWidth="1"/>
     <col min="9" max="9" width="16.83203125" customWidth="1"/>
     <col min="10" max="10" width="8.83203125" style="15"/>
   </cols>

</xml_diff>